<commit_message>
maven-metadata-generator-npm to version 0.2.56
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/bemonsteringsinstrument/bemonsteringsinstrument.xlsx
+++ b/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/bemonsteringsinstrument/bemonsteringsinstrument.xlsx
@@ -463,7 +463,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.collection.bemonsteringsinstrument.bemonsteringsinstrumenten</v>
       </c>
       <c r="D2" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E2" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermansteekbus|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualock|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualockpiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/avegaarbooras|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/balgpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/bovcentrifugaalpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/diamantboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandigepiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandiggeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpomp12v|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpompond|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubbelwandigekernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkleppomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandigepiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/edelmanboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkelwandigkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/geoprobe|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/graafmachine|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/grijpboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/hamerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/handboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorhsas|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorlin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kopeckysteekset100cm3|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kraan|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/lansboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/lepelboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/luchthamer|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/luchthevel|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/piston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/platavegaarboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsslang|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pvcaangescherpt30mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramguts|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutslin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutszlin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramkernboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ring|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/riversideboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/rollenbeitel|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/rvsstrooiselkader25cm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/schep|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/scheppot|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slagboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slangenpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spade|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spiraalboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spoelboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts20mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts25mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts30mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekhuls192cm3|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekhuls|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steenboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/strooiselkader|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/trilboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/tripkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/trippelwandigekernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vacuumpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/veenboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vibrocore|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/waterfles|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watermonsternemer|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watertrap|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigpomp</v>
@@ -513,7 +513,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ackermangedrukt</v>
       </c>
       <c r="D3" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E3" t="str">
         <v>null</v>
@@ -534,7 +534,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermansteekbus|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K3" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L3" t="str">
         <v>null</v>
@@ -563,7 +563,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ackermangeslagen</v>
       </c>
       <c r="D4" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E4" t="str">
         <v>null</v>
@@ -584,7 +584,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermansteekbus|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K4" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L4" t="str">
         <v>null</v>
@@ -613,7 +613,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ackermansteekbus</v>
       </c>
       <c r="D5" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E5" t="str">
         <v>null</v>
@@ -634,7 +634,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K5" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L5" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangeslagen</v>
@@ -663,7 +663,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.aqualock</v>
       </c>
       <c r="D6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E6" t="str">
         <v>null</v>
@@ -684,7 +684,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis</v>
       </c>
       <c r="K6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L6" t="str">
         <v>null</v>
@@ -713,7 +713,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.aqualockpiston</v>
       </c>
       <c r="D7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E7" t="str">
         <v>null</v>
@@ -734,7 +734,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/piston</v>
       </c>
       <c r="K7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L7" t="str">
         <v>null</v>
@@ -763,7 +763,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.avegaarbooras</v>
       </c>
       <c r="D8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E8" t="str">
         <v>null</v>
@@ -784,7 +784,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L8" t="str">
         <v>null</v>
@@ -813,7 +813,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.balgpomp</v>
       </c>
       <c r="D9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E9" t="str">
         <v>null</v>
@@ -834,7 +834,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp</v>
       </c>
       <c r="K9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L9" t="str">
         <v>null</v>
@@ -863,7 +863,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.boor</v>
       </c>
       <c r="D10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E10" t="str">
         <v>null</v>
@@ -884,7 +884,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/avegaarbooras|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/diamantboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/edelmanboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/geoprobe|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/grijpboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/hamerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/handboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorhsas|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorlin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/lansboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/lepelboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/luchthamer|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/luchthevel|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/platavegaarboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramguts|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutslin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutszlin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramkernboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/riversideboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/rollenbeitel|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slagboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spiraalboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spoelboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steenboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/trilboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/tripkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/veenboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vibrocore|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigerboor</v>
       </c>
       <c r="K10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L10" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/avegaarbooras|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/diamantboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/edelmanboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/geoprobe|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/grijpboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/hamerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/handboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorhsas|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/lansboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/lepelboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/luchthamer|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/luchthevel|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/platavegaarboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramguts|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/riversideboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/rollenbeitel|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slagboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spiraalboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/spoelboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steenboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/trilboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/veenboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vibrocore|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigerboor</v>
@@ -913,7 +913,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.bovcentrifugaalpomp</v>
       </c>
       <c r="D11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E11" t="str">
         <v>null</v>
@@ -934,7 +934,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigpomp</v>
       </c>
       <c r="K11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L11" t="str">
         <v>null</v>
@@ -963,7 +963,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.buis</v>
       </c>
       <c r="D12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E12" t="str">
         <v>null</v>
@@ -984,7 +984,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualock|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualockpiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandigepiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubbelwandigekernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandigepiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkelwandigkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/piston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pvcaangescherpt30mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/trippelwandigekernbuis</v>
       </c>
       <c r="K12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L12" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualock|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubbelwandigekernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkelwandigkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/piston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pvcaangescherpt30mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/trippelwandigekernbuis</v>
@@ -1013,7 +1013,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.diamantboor</v>
       </c>
       <c r="D13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E13" t="str">
         <v>null</v>
@@ -1034,7 +1034,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L13" t="str">
         <v>null</v>
@@ -1063,7 +1063,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dikwandig</v>
       </c>
       <c r="D14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E14" t="str">
         <v>null</v>
@@ -1084,7 +1084,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandiggeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L14" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandiggeslagen</v>
@@ -1113,7 +1113,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dikwandigepiston</v>
       </c>
       <c r="D15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E15" t="str">
         <v>null</v>
@@ -1134,7 +1134,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/piston</v>
       </c>
       <c r="K15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L15" t="str">
         <v>null</v>
@@ -1163,7 +1163,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dikwandiggeslagen</v>
       </c>
       <c r="D16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E16" t="str">
         <v>null</v>
@@ -1184,7 +1184,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L16" t="str">
         <v>null</v>
@@ -1213,7 +1213,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dompelpomp12v</v>
       </c>
       <c r="D17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E17" t="str">
         <v>null</v>
@@ -1234,7 +1234,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp</v>
       </c>
       <c r="K17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L17" t="str">
         <v>null</v>
@@ -1263,7 +1263,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dompelpompond</v>
       </c>
       <c r="D18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E18" t="str">
         <v>null</v>
@@ -1284,7 +1284,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp</v>
       </c>
       <c r="K18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L18" t="str">
         <v>null</v>
@@ -1313,7 +1313,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dubbelwandigekernbuis</v>
       </c>
       <c r="D19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E19" t="str">
         <v>null</v>
@@ -1334,7 +1334,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis</v>
       </c>
       <c r="K19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L19" t="str">
         <v>null</v>
@@ -1363,7 +1363,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dubkernbuis</v>
       </c>
       <c r="D20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E20" t="str">
         <v>null</v>
@@ -1384,7 +1384,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor</v>
       </c>
       <c r="K20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L20" t="str">
         <v>null</v>
@@ -1413,7 +1413,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dubkleppomp</v>
       </c>
       <c r="D21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E21" t="str">
         <v>null</v>
@@ -1434,7 +1434,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp</v>
       </c>
       <c r="K21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L21" t="str">
         <v>null</v>
@@ -1463,7 +1463,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dunwandig</v>
       </c>
       <c r="D22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E22" t="str">
         <v>null</v>
@@ -1484,7 +1484,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L22" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggeslagen</v>
@@ -1513,7 +1513,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dunwandigepiston</v>
       </c>
       <c r="D23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E23" t="str">
         <v>null</v>
@@ -1534,7 +1534,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/piston</v>
       </c>
       <c r="K23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L23" t="str">
         <v>null</v>
@@ -1563,7 +1563,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dunwandiggedrukt</v>
       </c>
       <c r="D24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E24" t="str">
         <v>null</v>
@@ -1584,7 +1584,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L24" t="str">
         <v>null</v>
@@ -1613,7 +1613,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.dunwandiggeslagen</v>
       </c>
       <c r="D25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E25" t="str">
         <v>null</v>
@@ -1634,7 +1634,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekbus</v>
       </c>
       <c r="K25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L25" t="str">
         <v>null</v>
@@ -1663,7 +1663,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.edelmanboor</v>
       </c>
       <c r="D26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E26" t="str">
         <v>null</v>
@@ -1684,7 +1684,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L26" t="str">
         <v>null</v>
@@ -1713,7 +1713,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.enkelwandigkernbuis</v>
       </c>
       <c r="D27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E27" t="str">
         <v>null</v>
@@ -1734,7 +1734,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis</v>
       </c>
       <c r="K27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L27" t="str">
         <v>null</v>
@@ -1763,7 +1763,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.enkkernbuis</v>
       </c>
       <c r="D28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E28" t="str">
         <v>null</v>
@@ -1784,7 +1784,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor</v>
       </c>
       <c r="K28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L28" t="str">
         <v>null</v>
@@ -1813,7 +1813,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.geoprobe</v>
       </c>
       <c r="D29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E29" t="str">
         <v>null</v>
@@ -1834,7 +1834,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L29" t="str">
         <v>null</v>
@@ -1863,7 +1863,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.graafmachine</v>
       </c>
       <c r="D30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E30" t="str">
         <v>null</v>
@@ -1884,7 +1884,7 @@
         <v>null</v>
       </c>
       <c r="K30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L30" t="str">
         <v>null</v>
@@ -1913,7 +1913,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.grijpboor</v>
       </c>
       <c r="D31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E31" t="str">
         <v>null</v>
@@ -1934,7 +1934,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L31" t="str">
         <v>null</v>
@@ -1963,7 +1963,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.hamerboor</v>
       </c>
       <c r="D32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E32" t="str">
         <v>null</v>
@@ -1984,7 +1984,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L32" t="str">
         <v>null</v>
@@ -2013,7 +2013,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.handboor</v>
       </c>
       <c r="D33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E33" t="str">
         <v>null</v>
@@ -2034,7 +2034,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L33" t="str">
         <v>null</v>
@@ -2063,7 +2063,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.holavegaarboorhsas</v>
       </c>
       <c r="D34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E34" t="str">
         <v>null</v>
@@ -2084,7 +2084,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorlin</v>
       </c>
       <c r="K34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L34" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorlin</v>
@@ -2113,7 +2113,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.holavegaarboorlin</v>
       </c>
       <c r="D35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E35" t="str">
         <v>null</v>
@@ -2134,7 +2134,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/holavegaarboorhsas</v>
       </c>
       <c r="K35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L35" t="str">
         <v>null</v>
@@ -2163,7 +2163,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.kerboor</v>
       </c>
       <c r="D36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E36" t="str">
         <v>null</v>
@@ -2184,7 +2184,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramkernboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/tripkernbuis</v>
       </c>
       <c r="K36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L36" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/enkkernbuis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramkernboor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/tripkernbuis</v>
@@ -2213,7 +2213,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.kopeckysteekset100cm3</v>
       </c>
       <c r="D37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E37" t="str">
         <v>null</v>
@@ -2234,7 +2234,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ring</v>
       </c>
       <c r="K37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L37" t="str">
         <v>null</v>
@@ -2263,7 +2263,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.kraan</v>
       </c>
       <c r="D38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E38" t="str">
         <v>null</v>
@@ -2284,7 +2284,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watermonsternemer</v>
       </c>
       <c r="K38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L38" t="str">
         <v>null</v>
@@ -2313,7 +2313,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.lansboor</v>
       </c>
       <c r="D39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E39" t="str">
         <v>null</v>
@@ -2334,7 +2334,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L39" t="str">
         <v>null</v>
@@ -2363,7 +2363,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.lepelboor</v>
       </c>
       <c r="D40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E40" t="str">
         <v>null</v>
@@ -2384,7 +2384,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L40" t="str">
         <v>null</v>
@@ -2413,7 +2413,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.luchthamer</v>
       </c>
       <c r="D41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E41" t="str">
         <v>null</v>
@@ -2434,7 +2434,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L41" t="str">
         <v>null</v>
@@ -2463,7 +2463,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.luchthevel</v>
       </c>
       <c r="D42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E42" t="str">
         <v>null</v>
@@ -2484,7 +2484,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L42" t="str">
         <v>null</v>
@@ -2513,7 +2513,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.perspomp</v>
       </c>
       <c r="D43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E43" t="str">
         <v>null</v>
@@ -2534,7 +2534,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/balgpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpomp12v|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpompond|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkleppomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsslang</v>
       </c>
       <c r="K43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L43" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/balgpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpomp12v|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpompond|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkleppomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsslang</v>
@@ -2563,7 +2563,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.piston</v>
       </c>
       <c r="D44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E44" t="str">
         <v>null</v>
@@ -2584,7 +2584,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualockpiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandigepiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandigepiston</v>
       </c>
       <c r="K44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L44" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/aqualockpiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandigepiston|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandigepiston</v>
@@ -2613,7 +2613,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.platavegaarboor</v>
       </c>
       <c r="D45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E45" t="str">
         <v>null</v>
@@ -2634,7 +2634,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L45" t="str">
         <v>null</v>
@@ -2663,7 +2663,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.pomp</v>
       </c>
       <c r="D46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E46" t="str">
         <v>null</v>
@@ -2684,7 +2684,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/balgpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/bovcentrifugaalpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpomp12v|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dompelpompond|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dubkleppomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pulsslang|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slangenpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vacuumpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigpomp</v>
       </c>
       <c r="K46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L46" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigpomp</v>
@@ -2713,7 +2713,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.pulsboor</v>
       </c>
       <c r="D47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E47" t="str">
         <v>null</v>
@@ -2734,7 +2734,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L47" t="str">
         <v>null</v>
@@ -2763,7 +2763,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.pulsslang</v>
       </c>
       <c r="D48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E48" t="str">
         <v>null</v>
@@ -2784,7 +2784,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/perspomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp</v>
       </c>
       <c r="K48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L48" t="str">
         <v>null</v>
@@ -2813,7 +2813,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.pvcaangescherpt30mm</v>
       </c>
       <c r="D49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E49" t="str">
         <v>null</v>
@@ -2834,7 +2834,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis</v>
       </c>
       <c r="K49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L49" t="str">
         <v>null</v>
@@ -2863,7 +2863,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ramguts</v>
       </c>
       <c r="D50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E50" t="str">
         <v>null</v>
@@ -2884,7 +2884,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutslin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutszlin</v>
       </c>
       <c r="K50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L50" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutslin|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramgutszlin</v>
@@ -2913,7 +2913,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ramgutslin</v>
       </c>
       <c r="D51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E51" t="str">
         <v>null</v>
@@ -2934,7 +2934,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramguts</v>
       </c>
       <c r="K51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L51" t="str">
         <v>null</v>
@@ -2963,7 +2963,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ramgutszlin</v>
       </c>
       <c r="D52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E52" t="str">
         <v>null</v>
@@ -2984,7 +2984,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ramguts</v>
       </c>
       <c r="K52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L52" t="str">
         <v>null</v>
@@ -3013,7 +3013,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ramkernboor</v>
       </c>
       <c r="D53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E53" t="str">
         <v>null</v>
@@ -3034,7 +3034,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor</v>
       </c>
       <c r="K53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L53" t="str">
         <v>null</v>
@@ -3063,7 +3063,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.ring</v>
       </c>
       <c r="D54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E54" t="str">
         <v>null</v>
@@ -3084,7 +3084,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kopeckysteekset100cm3</v>
       </c>
       <c r="K54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L54" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kopeckysteekset100cm3</v>
@@ -3113,7 +3113,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.riversideboor</v>
       </c>
       <c r="D55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E55" t="str">
         <v>null</v>
@@ -3134,7 +3134,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L55" t="str">
         <v>null</v>
@@ -3163,7 +3163,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.rollenbeitel</v>
       </c>
       <c r="D56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E56" t="str">
         <v>null</v>
@@ -3184,7 +3184,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L56" t="str">
         <v>null</v>
@@ -3213,7 +3213,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.rvsstrooiselkader25cm</v>
       </c>
       <c r="D57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E57" t="str">
         <v>null</v>
@@ -3234,7 +3234,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/strooiselkader</v>
       </c>
       <c r="K57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L57" t="str">
         <v>null</v>
@@ -3263,7 +3263,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.schep</v>
       </c>
       <c r="D58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E58" t="str">
         <v>null</v>
@@ -3284,7 +3284,7 @@
         <v>null</v>
       </c>
       <c r="K58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L58" t="str">
         <v>null</v>
@@ -3313,7 +3313,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.scheppot</v>
       </c>
       <c r="D59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E59" t="str">
         <v>null</v>
@@ -3334,7 +3334,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watermonsternemer</v>
       </c>
       <c r="K59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L59" t="str">
         <v>null</v>
@@ -3363,7 +3363,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.slagboor</v>
       </c>
       <c r="D60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E60" t="str">
         <v>null</v>
@@ -3384,7 +3384,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L60" t="str">
         <v>null</v>
@@ -3413,7 +3413,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.slangenpomp</v>
       </c>
       <c r="D61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E61" t="str">
         <v>null</v>
@@ -3434,7 +3434,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigpomp</v>
       </c>
       <c r="K61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L61" t="str">
         <v>null</v>
@@ -3463,7 +3463,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.spade</v>
       </c>
       <c r="D62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E62" t="str">
         <v>null</v>
@@ -3484,7 +3484,7 @@
         <v>null</v>
       </c>
       <c r="K62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L62" t="str">
         <v>null</v>
@@ -3513,7 +3513,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.spiraalboor</v>
       </c>
       <c r="D63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E63" t="str">
         <v>null</v>
@@ -3534,7 +3534,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L63" t="str">
         <v>null</v>
@@ -3563,7 +3563,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.spoelboor</v>
       </c>
       <c r="D64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E64" t="str">
         <v>null</v>
@@ -3584,7 +3584,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L64" t="str">
         <v>null</v>
@@ -3613,7 +3613,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekbus</v>
       </c>
       <c r="D65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E65" t="str">
         <v>null</v>
@@ -3634,7 +3634,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermangeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermansteekbus|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandiggeslagen|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggedrukt|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandiggeslagen</v>
       </c>
       <c r="K65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L65" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/ackermansteekbus|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dikwandig|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/dunwandig</v>
@@ -3663,7 +3663,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekguts</v>
       </c>
       <c r="D66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E66" t="str">
         <v>null</v>
@@ -3684,7 +3684,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts20mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts25mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts30mm</v>
       </c>
       <c r="K66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L66" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts20mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts25mm|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts30mm</v>
@@ -3713,7 +3713,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekguts20mm</v>
       </c>
       <c r="D67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E67" t="str">
         <v>null</v>
@@ -3734,7 +3734,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts</v>
       </c>
       <c r="K67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L67" t="str">
         <v>null</v>
@@ -3763,7 +3763,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekguts25mm</v>
       </c>
       <c r="D68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E68" t="str">
         <v>null</v>
@@ -3784,7 +3784,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts</v>
       </c>
       <c r="K68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L68" t="str">
         <v>null</v>
@@ -3813,7 +3813,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekguts30mm</v>
       </c>
       <c r="D69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E69" t="str">
         <v>null</v>
@@ -3834,7 +3834,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekguts</v>
       </c>
       <c r="K69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L69" t="str">
         <v>null</v>
@@ -3863,7 +3863,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekhuls</v>
       </c>
       <c r="D70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E70" t="str">
         <v>null</v>
@@ -3884,7 +3884,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekhuls192cm3</v>
       </c>
       <c r="K70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L70" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekhuls192cm3</v>
@@ -3913,7 +3913,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steekhuls192cm3</v>
       </c>
       <c r="D71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E71" t="str">
         <v>null</v>
@@ -3934,7 +3934,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/steekhuls</v>
       </c>
       <c r="K71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L71" t="str">
         <v>null</v>
@@ -3963,7 +3963,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.steenboor</v>
       </c>
       <c r="D72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E72" t="str">
         <v>null</v>
@@ -3984,7 +3984,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L72" t="str">
         <v>null</v>
@@ -4013,7 +4013,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.strooiselkader</v>
       </c>
       <c r="D73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E73" t="str">
         <v>null</v>
@@ -4034,7 +4034,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/rvsstrooiselkader25cm</v>
       </c>
       <c r="K73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L73" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/rvsstrooiselkader25cm</v>
@@ -4063,7 +4063,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.trilboor</v>
       </c>
       <c r="D74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E74" t="str">
         <v>null</v>
@@ -4084,7 +4084,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L74" t="str">
         <v>null</v>
@@ -4113,7 +4113,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.tripkernbuis</v>
       </c>
       <c r="D75" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E75" t="str">
         <v>null</v>
@@ -4134,7 +4134,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kerboor</v>
       </c>
       <c r="K75" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L75" t="str">
         <v>null</v>
@@ -4163,7 +4163,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.trippelwandigekernbuis</v>
       </c>
       <c r="D76" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E76" t="str">
         <v>null</v>
@@ -4184,7 +4184,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/buis</v>
       </c>
       <c r="K76" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L76" t="str">
         <v>null</v>
@@ -4213,7 +4213,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.vacuumpomp</v>
       </c>
       <c r="D77" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E77" t="str">
         <v>null</v>
@@ -4234,7 +4234,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/zuigpomp</v>
       </c>
       <c r="K77" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L77" t="str">
         <v>null</v>
@@ -4263,7 +4263,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.veenboor</v>
       </c>
       <c r="D78" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E78" t="str">
         <v>null</v>
@@ -4284,7 +4284,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K78" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L78" t="str">
         <v>null</v>
@@ -4313,7 +4313,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.vibrocore</v>
       </c>
       <c r="D79" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E79" t="str">
         <v>null</v>
@@ -4334,7 +4334,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K79" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L79" t="str">
         <v>null</v>
@@ -4363,7 +4363,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.waterfles</v>
       </c>
       <c r="D80" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E80" t="str">
         <v>null</v>
@@ -4384,7 +4384,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watermonsternemer</v>
       </c>
       <c r="K80" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L80" t="str">
         <v>null</v>
@@ -4413,7 +4413,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.watermonsternemer</v>
       </c>
       <c r="D81" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E81" t="str">
         <v>null</v>
@@ -4434,7 +4434,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kraan|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/scheppot|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/waterfles|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watertrap</v>
       </c>
       <c r="K81" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L81" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/kraan|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/scheppot|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/waterfles|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watertrap</v>
@@ -4463,7 +4463,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.watertrap</v>
       </c>
       <c r="D82" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E82" t="str">
         <v>null</v>
@@ -4484,7 +4484,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/watermonsternemer</v>
       </c>
       <c r="K82" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L82" t="str">
         <v>null</v>
@@ -4513,7 +4513,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.zuigboor</v>
       </c>
       <c r="D83" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E83" t="str">
         <v>null</v>
@@ -4534,7 +4534,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K83" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L83" t="str">
         <v>null</v>
@@ -4563,7 +4563,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.zuigerboor</v>
       </c>
       <c r="D84" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E84" t="str">
         <v>null</v>
@@ -4584,7 +4584,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/boor</v>
       </c>
       <c r="K84" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L84" t="str">
         <v>null</v>
@@ -4613,7 +4613,7 @@
         <v>be.vlaanderen.bodemenondergrond.data.id.concept.bemonsteringsinstrument.zuigpomp</v>
       </c>
       <c r="D85" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="E85" t="str">
         <v>null</v>
@@ -4634,7 +4634,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/bovcentrifugaalpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/pomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slangenpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vacuumpomp</v>
       </c>
       <c r="K85" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="L85" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/bovcentrifugaalpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/slangenpomp|https://data.bodemenondergrond.vlaanderen.be/id/concept/bemonsteringsinstrument/vacuumpomp</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bemonsteringsinstrument</v>
       </c>
       <c r="B86" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>

</xml_diff>